<commit_message>
Coordenadas, cambios en los tests y documentación
</commit_message>
<xml_diff>
--- a/ExcelExporter.Tests/Test.xlsx
+++ b/ExcelExporter.Tests/Test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="ExistingHoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -392,7 +392,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>